<commit_message>
Revised nested programs to provide synergistic impacts
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_malaria.xlsx
+++ b/tests/frameworks/framework_malaria.xlsx
@@ -4454,10 +4454,10 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G52" sqref="G52"/>
+      <selection pane="bottomRight" activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5009,7 +5009,7 @@
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
       <c r="H17" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>7</v>
@@ -5039,7 +5039,7 @@
       <c r="F18" s="36"/>
       <c r="G18" s="36"/>
       <c r="H18" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>7</v>
@@ -5668,7 +5668,7 @@
         <v>194</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>7</v>
@@ -5698,7 +5698,7 @@
         <v>195</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>7</v>
@@ -5897,7 +5897,7 @@
         <v>197</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>7</v>
@@ -5926,7 +5926,7 @@
         <v>198</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>7</v>

</xml_diff>